<commit_message>
File reading now working
</commit_message>
<xml_diff>
--- a/resources/manifests/1.1/manifest.example.xlsx
+++ b/resources/manifests/1.1/manifest.example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hjjoshi/dev/ms-checker/resources/manifests/1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330BD2C8-46DB-C24B-AE9B-1EC2E29A6A5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690B2BBA-EBAA-F741-ADFB-B8042A29B8F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7100" yWindow="4600" windowWidth="27300" windowHeight="18340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,7 +645,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>